<commit_message>
data corrected: regtime now after borntime (script updated)
</commit_message>
<xml_diff>
--- a/quanlythuvien/data/List_DocGia.xlsx
+++ b/quanlythuvien/data/List_DocGia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\New folder (2)\mini-library-manager\quanlythuvien\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407D61CE-B6E5-4333-B2E0-5A099F9F8742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9129CEB4-73D7-4658-ACA5-2BCD0A956AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3DFCDBD6-3BA2-458F-9082-1DA170B60CF4}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="826">
   <si>
     <t>username</t>
   </si>
@@ -2077,6 +2077,450 @@
   </si>
   <si>
     <t>Huynh Le Bang</t>
+  </si>
+  <si>
+    <t>16/03/2006 10:26:12</t>
+  </si>
+  <si>
+    <t>30/09/1981 13:35:32</t>
+  </si>
+  <si>
+    <t>21/11/1991 11:13:21</t>
+  </si>
+  <si>
+    <t>30/03/1993 09:29:37</t>
+  </si>
+  <si>
+    <t>19/03/1983 01:52:07</t>
+  </si>
+  <si>
+    <t>21/08/2007 10:43:14</t>
+  </si>
+  <si>
+    <t>21/11/1989 20:26:03</t>
+  </si>
+  <si>
+    <t>15/09/1980 11:04:19</t>
+  </si>
+  <si>
+    <t>28/12/1993 11:59:16</t>
+  </si>
+  <si>
+    <t>16/07/2009 05:19:46</t>
+  </si>
+  <si>
+    <t>27/06/1986 01:45:48</t>
+  </si>
+  <si>
+    <t>24/07/2006 03:31:51</t>
+  </si>
+  <si>
+    <t>15/06/1984 03:50:29</t>
+  </si>
+  <si>
+    <t>23/08/2003 19:24:05</t>
+  </si>
+  <si>
+    <t>30/07/2005 22:31:58</t>
+  </si>
+  <si>
+    <t>21/03/2007 01:55:55</t>
+  </si>
+  <si>
+    <t>29/12/2004 23:35:04</t>
+  </si>
+  <si>
+    <t>13/11/1981 13:46:42</t>
+  </si>
+  <si>
+    <t>23/01/2003 11:02:29</t>
+  </si>
+  <si>
+    <t>13/01/2004 20:32:53</t>
+  </si>
+  <si>
+    <t>16/10/1980 12:29:50</t>
+  </si>
+  <si>
+    <t>15/01/2008 14:03:45</t>
+  </si>
+  <si>
+    <t>19/02/1994 22:40:35</t>
+  </si>
+  <si>
+    <t>23/05/2008 23:58:58</t>
+  </si>
+  <si>
+    <t>27/11/1995 05:15:49</t>
+  </si>
+  <si>
+    <t>17/04/2006 13:55:30</t>
+  </si>
+  <si>
+    <t>13/11/1996 08:16:16</t>
+  </si>
+  <si>
+    <t>31/08/1984 18:59:00</t>
+  </si>
+  <si>
+    <t>21/03/1996 22:26:09</t>
+  </si>
+  <si>
+    <t>25/09/2008 09:32:26</t>
+  </si>
+  <si>
+    <t>22/11/1997 22:26:19</t>
+  </si>
+  <si>
+    <t>22/07/1998 17:53:01</t>
+  </si>
+  <si>
+    <t>30/10/1985 13:05:22</t>
+  </si>
+  <si>
+    <t>30/12/2004 00:12:02</t>
+  </si>
+  <si>
+    <t>30/08/2009 13:48:51</t>
+  </si>
+  <si>
+    <t>25/08/1992 20:22:49</t>
+  </si>
+  <si>
+    <t>24/10/1981 10:28:00</t>
+  </si>
+  <si>
+    <t>24/06/1996 17:11:48</t>
+  </si>
+  <si>
+    <t>28/08/1985 14:49:09</t>
+  </si>
+  <si>
+    <t>25/02/2003 16:23:17</t>
+  </si>
+  <si>
+    <t>30/06/2006 23:38:14</t>
+  </si>
+  <si>
+    <t>29/10/2004 22:11:59</t>
+  </si>
+  <si>
+    <t>19/06/1990 05:52:05</t>
+  </si>
+  <si>
+    <t>28/08/1984 05:56:07</t>
+  </si>
+  <si>
+    <t>24/03/2007 15:40:15</t>
+  </si>
+  <si>
+    <t>27/12/1984 04:25:50</t>
+  </si>
+  <si>
+    <t>24/04/1992 07:13:50</t>
+  </si>
+  <si>
+    <t>13/11/1991 18:56:40</t>
+  </si>
+  <si>
+    <t>22/03/2003 13:26:36</t>
+  </si>
+  <si>
+    <t>27/04/1992 09:58:29</t>
+  </si>
+  <si>
+    <t>17/12/1980 07:52:04</t>
+  </si>
+  <si>
+    <t>25/12/1995 13:49:43</t>
+  </si>
+  <si>
+    <t>23/08/2000 11:29:09</t>
+  </si>
+  <si>
+    <t>25/06/1994 03:52:19</t>
+  </si>
+  <si>
+    <t>31/03/1981 12:45:38</t>
+  </si>
+  <si>
+    <t>22/05/1986 04:15:37</t>
+  </si>
+  <si>
+    <t>31/07/1980 08:21:43</t>
+  </si>
+  <si>
+    <t>31/08/1995 11:11:01</t>
+  </si>
+  <si>
+    <t>19/11/2007 14:46:58</t>
+  </si>
+  <si>
+    <t>25/09/1989 09:17:13</t>
+  </si>
+  <si>
+    <t>15/12/1997 11:25:47</t>
+  </si>
+  <si>
+    <t>18/11/1988 05:16:32</t>
+  </si>
+  <si>
+    <t>30/01/1993 11:28:48</t>
+  </si>
+  <si>
+    <t>21/01/1993 02:17:25</t>
+  </si>
+  <si>
+    <t>19/06/1991 21:06:56</t>
+  </si>
+  <si>
+    <t>15/06/2004 08:22:30</t>
+  </si>
+  <si>
+    <t>16/07/2008 17:45:08</t>
+  </si>
+  <si>
+    <t>16/12/1984 10:47:41</t>
+  </si>
+  <si>
+    <t>16/05/2007 09:05:17</t>
+  </si>
+  <si>
+    <t>28/04/1985 23:53:15</t>
+  </si>
+  <si>
+    <t>13/06/1995 19:31:29</t>
+  </si>
+  <si>
+    <t>19/05/2007 09:47:43</t>
+  </si>
+  <si>
+    <t>25/05/2000 10:01:36</t>
+  </si>
+  <si>
+    <t>26/10/2005 12:37:35</t>
+  </si>
+  <si>
+    <t>19/08/1986 05:40:35</t>
+  </si>
+  <si>
+    <t>26/12/1999 12:33:59</t>
+  </si>
+  <si>
+    <t>15/11/1987 06:44:06</t>
+  </si>
+  <si>
+    <t>21/05/2008 14:42:18</t>
+  </si>
+  <si>
+    <t>27/07/2006 19:01:30</t>
+  </si>
+  <si>
+    <t>25/04/1987 10:40:21</t>
+  </si>
+  <si>
+    <t>25/02/1997 14:20:12</t>
+  </si>
+  <si>
+    <t>21/05/2003 23:30:27</t>
+  </si>
+  <si>
+    <t>23/11/2003 22:16:29</t>
+  </si>
+  <si>
+    <t>15/06/1998 16:04:38</t>
+  </si>
+  <si>
+    <t>26/09/1999 17:25:45</t>
+  </si>
+  <si>
+    <t>24/05/1993 08:09:01</t>
+  </si>
+  <si>
+    <t>31/03/2008 14:59:29</t>
+  </si>
+  <si>
+    <t>27/09/1993 19:38:31</t>
+  </si>
+  <si>
+    <t>25/03/2008 11:59:28</t>
+  </si>
+  <si>
+    <t>23/01/1989 03:24:24</t>
+  </si>
+  <si>
+    <t>20/08/1998 09:43:21</t>
+  </si>
+  <si>
+    <t>24/09/1995 02:34:37</t>
+  </si>
+  <si>
+    <t>21/07/2010 05:05:25</t>
+  </si>
+  <si>
+    <t>21/03/1982 13:16:56</t>
+  </si>
+  <si>
+    <t>24/01/2001 02:18:27</t>
+  </si>
+  <si>
+    <t>21/03/1983 14:46:59</t>
+  </si>
+  <si>
+    <t>17/07/2006 09:50:51</t>
+  </si>
+  <si>
+    <t>21/04/1981 04:54:51</t>
+  </si>
+  <si>
+    <t>24/06/1999 19:06:17</t>
+  </si>
+  <si>
+    <t>18/10/1980 01:28:23</t>
+  </si>
+  <si>
+    <t>14/10/1989 11:59:48</t>
+  </si>
+  <si>
+    <t>19/09/1999 10:22:31</t>
+  </si>
+  <si>
+    <t>17/01/2009 09:26:19</t>
+  </si>
+  <si>
+    <t>15/01/2001 17:57:40</t>
+  </si>
+  <si>
+    <t>25/04/1995 06:42:23</t>
+  </si>
+  <si>
+    <t>14/04/1980 18:17:46</t>
+  </si>
+  <si>
+    <t>14/07/2006 23:51:08</t>
+  </si>
+  <si>
+    <t>21/09/1998 10:21:51</t>
+  </si>
+  <si>
+    <t>31/12/1986 16:10:34</t>
+  </si>
+  <si>
+    <t>20/08/1988 07:18:21</t>
+  </si>
+  <si>
+    <t>13/10/1999 09:57:37</t>
+  </si>
+  <si>
+    <t>19/05/1998 16:35:13</t>
+  </si>
+  <si>
+    <t>27/09/1999 15:12:45</t>
+  </si>
+  <si>
+    <t>19/08/1986 12:42:10</t>
+  </si>
+  <si>
+    <t>28/05/1990 09:30:08</t>
+  </si>
+  <si>
+    <t>15/09/1985 06:34:32</t>
+  </si>
+  <si>
+    <t>26/10/1994 23:58:14</t>
+  </si>
+  <si>
+    <t>13/01/1982 11:31:33</t>
+  </si>
+  <si>
+    <t>14/12/1997 02:22:44</t>
+  </si>
+  <si>
+    <t>24/05/2002 04:41:30</t>
+  </si>
+  <si>
+    <t>22/06/2001 02:17:50</t>
+  </si>
+  <si>
+    <t>21/08/2009 10:10:20</t>
+  </si>
+  <si>
+    <t>24/10/2009 05:19:02</t>
+  </si>
+  <si>
+    <t>30/07/2007 17:09:43</t>
+  </si>
+  <si>
+    <t>18/03/2007 14:03:57</t>
+  </si>
+  <si>
+    <t>14/08/1994 13:44:10</t>
+  </si>
+  <si>
+    <t>23/11/2008 22:10:23</t>
+  </si>
+  <si>
+    <t>25/10/2006 12:40:51</t>
+  </si>
+  <si>
+    <t>21/07/1999 12:34:13</t>
+  </si>
+  <si>
+    <t>22/12/2002 07:13:07</t>
+  </si>
+  <si>
+    <t>31/05/1988 10:04:10</t>
+  </si>
+  <si>
+    <t>27/11/1981 04:10:37</t>
+  </si>
+  <si>
+    <t>22/11/2008 18:39:48</t>
+  </si>
+  <si>
+    <t>21/03/1994 06:59:44</t>
+  </si>
+  <si>
+    <t>17/08/2010 14:56:09</t>
+  </si>
+  <si>
+    <t>19/07/1984 23:20:45</t>
+  </si>
+  <si>
+    <t>20/11/2002 00:50:31</t>
+  </si>
+  <si>
+    <t>20/03/2001 18:32:34</t>
+  </si>
+  <si>
+    <t>21/07/1982 19:53:15</t>
+  </si>
+  <si>
+    <t>22/05/1995 05:05:35</t>
+  </si>
+  <si>
+    <t>17/07/2003 22:12:33</t>
+  </si>
+  <si>
+    <t>16/04/1995 07:42:32</t>
+  </si>
+  <si>
+    <t>15/06/2000 09:32:40</t>
+  </si>
+  <si>
+    <t>22/12/1991 08:14:34</t>
+  </si>
+  <si>
+    <t>28/01/1990 15:51:46</t>
+  </si>
+  <si>
+    <t>30/09/1998 07:14:39</t>
+  </si>
+  <si>
+    <t>28/01/2003 03:07:46</t>
+  </si>
+  <si>
+    <t>22/07/2001 04:29:20</t>
   </si>
 </sst>
 </file>
@@ -2463,8 +2907,8 @@
   <dimension ref="A1:H119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,11 +2958,11 @@
       <c r="C2" t="s">
         <v>560</v>
       </c>
-      <c r="D2" s="1">
-        <v>38792.434859175955</v>
-      </c>
-      <c r="E2" s="1">
-        <v>29859.566346948694</v>
+      <c r="D2" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>679</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>324</v>
@@ -2541,10 +2985,10 @@
         <v>561</v>
       </c>
       <c r="D3" s="1">
-        <v>33563.467604438956</v>
-      </c>
-      <c r="E3" s="1">
-        <v>36139.104928228036</v>
+        <v>36080.104930555557</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>680</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>326</v>
@@ -2566,11 +3010,11 @@
       <c r="C4" t="s">
         <v>562</v>
       </c>
-      <c r="D4" s="1">
-        <v>34058.395570023706</v>
-      </c>
-      <c r="E4" s="1">
-        <v>30394.077858748715</v>
+      <c r="D4" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>682</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>328</v>
@@ -2593,10 +3037,10 @@
         <v>563</v>
       </c>
       <c r="D5" s="1">
-        <v>40157.120447416462</v>
-      </c>
-      <c r="E5" s="1">
-        <v>39315.446689491277</v>
+        <v>40098.120451388888</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>683</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>330</v>
@@ -2618,11 +3062,11 @@
       <c r="C6" t="s">
         <v>564</v>
       </c>
-      <c r="D6" s="1">
-        <v>32833.85142346553</v>
+      <c r="D6" s="1" t="s">
+        <v>684</v>
       </c>
       <c r="E6" s="1">
-        <v>30808.082287530578</v>
+        <v>30838.082291666666</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>332</v>
@@ -2645,10 +3089,10 @@
         <v>565</v>
       </c>
       <c r="D7" s="1">
-        <v>29479.461326271696</v>
-      </c>
-      <c r="E7" s="1">
-        <v>34281.37624683886</v>
+        <v>34192.376250000001</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>685</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>334</v>
@@ -2671,10 +3115,10 @@
         <v>566</v>
       </c>
       <c r="D8" s="1">
-        <v>35888.397591075351</v>
-      </c>
-      <c r="E8" s="1">
-        <v>34331.499490778224</v>
+        <v>35858.397592592592</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>686</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>336</v>
@@ -2697,10 +3141,10 @@
         <v>567</v>
       </c>
       <c r="D9" s="1">
-        <v>35013.083082238103</v>
+        <v>34983.083078703705</v>
       </c>
       <c r="E9" s="1">
-        <v>33055.500720348631</v>
+        <v>32880.500717592593</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>338</v>
@@ -2722,11 +3166,11 @@
       <c r="C10" t="s">
         <v>568</v>
       </c>
-      <c r="D10" s="1">
-        <v>40010.22206142504</v>
-      </c>
-      <c r="E10" s="1">
-        <v>31590.073474651388</v>
+      <c r="D10" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>688</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>340</v>
@@ -2748,11 +3192,11 @@
       <c r="C11" t="s">
         <v>569</v>
       </c>
-      <c r="D11" s="1">
-        <v>38922.147122674141</v>
-      </c>
-      <c r="E11" s="1">
-        <v>30848.160058760026</v>
+      <c r="D11" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>690</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>342</v>
@@ -2775,10 +3219,10 @@
         <v>570</v>
       </c>
       <c r="D12" s="1">
-        <v>30077.95293236605</v>
+        <v>37750.8512962963</v>
       </c>
       <c r="E12" s="1">
-        <v>37869.851298341404</v>
+        <v>30107.952928240742</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>344</v>
@@ -2800,11 +3244,11 @@
       <c r="C13" t="s">
         <v>571</v>
       </c>
-      <c r="D13" s="1">
-        <v>35886.335328391942</v>
+      <c r="D13" s="1" t="s">
+        <v>691</v>
       </c>
       <c r="E13" s="1">
-        <v>37856.808393353014</v>
+        <v>35799.335324074076</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>346</v>
@@ -2826,11 +3270,11 @@
       <c r="C14" t="s">
         <v>572</v>
       </c>
-      <c r="D14" s="1">
-        <v>33793.857696036466</v>
+      <c r="D14" s="1" t="s">
+        <v>692</v>
       </c>
       <c r="E14" s="1">
-        <v>38563.938862495583</v>
+        <v>33823.85769675926</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>348</v>
@@ -2852,11 +3296,11 @@
       <c r="C15" t="s">
         <v>573</v>
       </c>
-      <c r="D15" s="1">
-        <v>39162.080496590039</v>
-      </c>
-      <c r="E15" s="1">
-        <v>38350.982683614202</v>
+      <c r="D15" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>694</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>350</v>
@@ -2879,10 +3323,10 @@
         <v>574</v>
       </c>
       <c r="D16" s="1">
-        <v>38355.722365927002</v>
-      </c>
-      <c r="E16" s="1">
-        <v>29903.574102124003</v>
+        <v>38412.722361111111</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>695</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>352</v>
@@ -2905,10 +3349,10 @@
         <v>575</v>
       </c>
       <c r="D17" s="1">
-        <v>37644.460053245333</v>
-      </c>
-      <c r="E17" s="1">
-        <v>38964.958739595648</v>
+        <v>38816.958738425928</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>696</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>354</v>
@@ -2930,11 +3374,11 @@
       <c r="C18" t="s">
         <v>576</v>
       </c>
-      <c r="D18" s="1">
-        <v>31292.589481006547</v>
+      <c r="D18" s="1" t="s">
+        <v>697</v>
       </c>
       <c r="E18" s="1">
-        <v>37999.856168630322</v>
+        <v>31087.589479166665</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>356</v>
@@ -2957,10 +3401,10 @@
         <v>577</v>
       </c>
       <c r="D19" s="1">
-        <v>36987.830057927844</v>
+        <v>37046.830057870371</v>
       </c>
       <c r="E19" s="1">
-        <v>30508.820764501481</v>
+        <v>30627.820763888889</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>358</v>
@@ -2983,10 +3427,10 @@
         <v>578</v>
       </c>
       <c r="D20" s="1">
-        <v>33673.041849837435</v>
-      </c>
-      <c r="E20" s="1">
-        <v>29510.520715369021</v>
+        <v>33880.041851851849</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>698</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>360</v>
@@ -3009,10 +3453,10 @@
         <v>579</v>
       </c>
       <c r="D21" s="1">
-        <v>30844.753396215438</v>
+        <v>30992.753391203703</v>
       </c>
       <c r="E21" s="1">
-        <v>29533.004488631224</v>
+        <v>29444.004490740739</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>362</v>
@@ -3034,11 +3478,11 @@
       <c r="C22" t="s">
         <v>580</v>
       </c>
-      <c r="D22" s="1">
-        <v>34585.212235493287</v>
+      <c r="D22" s="1" t="s">
+        <v>699</v>
       </c>
       <c r="E22" s="1">
-        <v>39462.585938010918</v>
+        <v>34555.212233796294</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>364</v>
@@ -3061,10 +3505,10 @@
         <v>581</v>
       </c>
       <c r="D23" s="1">
-        <v>39032.373844296999</v>
-      </c>
-      <c r="E23" s="1">
-        <v>34384.944844617392</v>
+        <v>39032.373842592591</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>700</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>366</v>
@@ -3086,11 +3530,11 @@
       <c r="C24" t="s">
         <v>582</v>
       </c>
-      <c r="D24" s="1">
-        <v>35030.219311389847</v>
-      </c>
-      <c r="E24" s="1">
-        <v>39591.999288050094</v>
+      <c r="D24" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>702</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>368</v>
@@ -3112,11 +3556,11 @@
       <c r="C25" t="s">
         <v>583</v>
       </c>
-      <c r="D25" s="1">
-        <v>29992.422755342101</v>
+      <c r="D25" s="1" t="s">
+        <v>703</v>
       </c>
       <c r="E25" s="1">
-        <v>38824.580214012392</v>
+        <v>30226.422754629628</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>370</v>
@@ -3138,11 +3582,11 @@
       <c r="C26" t="s">
         <v>584</v>
       </c>
-      <c r="D26" s="1">
-        <v>35382.34463364246</v>
-      </c>
-      <c r="E26" s="1">
-        <v>30925.790969411042</v>
+      <c r="D26" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>705</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>372</v>
@@ -3165,10 +3609,10 @@
         <v>585</v>
       </c>
       <c r="D27" s="1">
-        <v>35348.964365045686</v>
-      </c>
-      <c r="E27" s="1">
-        <v>35145.934825423639</v>
+        <v>35348.964363425926</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>706</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>374</v>
@@ -3190,11 +3634,11 @@
       <c r="C28" t="s">
         <v>586</v>
       </c>
-      <c r="D28" s="1">
-        <v>39716.397517867052</v>
-      </c>
-      <c r="E28" s="1">
-        <v>35756.934945168818</v>
+      <c r="D28" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>708</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>376</v>
@@ -3216,11 +3660,11 @@
       <c r="C29" t="s">
         <v>587</v>
       </c>
-      <c r="D29" s="1">
-        <v>35998.745146884547</v>
-      </c>
-      <c r="E29" s="1">
-        <v>31350.545392990389</v>
+      <c r="D29" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>710</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>378</v>
@@ -3242,11 +3686,11 @@
       <c r="C30" t="s">
         <v>588</v>
       </c>
-      <c r="D30" s="1">
-        <v>38351.008356399791</v>
+      <c r="D30" s="1" t="s">
+        <v>711</v>
       </c>
       <c r="E30" s="1">
-        <v>36655.874892092987</v>
+        <v>36774.874895833331</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>380</v>
@@ -3268,11 +3712,11 @@
       <c r="C31" t="s">
         <v>589</v>
       </c>
-      <c r="D31" s="1">
-        <v>40055.575590248089</v>
+      <c r="D31" s="1" t="s">
+        <v>712</v>
       </c>
       <c r="E31" s="1">
-        <v>33736.654962021887</v>
+        <v>33943.654965277776</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>382</v>
@@ -3294,11 +3738,11 @@
       <c r="C32" t="s">
         <v>590</v>
       </c>
-      <c r="D32" s="1">
-        <v>29883.436106204015</v>
-      </c>
-      <c r="E32" s="1">
-        <v>33841.84917534476</v>
+      <c r="D32" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>714</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>384</v>
@@ -3320,11 +3764,11 @@
       <c r="C33" t="s">
         <v>591</v>
       </c>
-      <c r="D33" s="1">
-        <v>35007.343411651098</v>
+      <c r="D33" s="1" t="s">
+        <v>715</v>
       </c>
       <c r="E33" s="1">
-        <v>35240.716524429939</v>
+        <v>34800.343414351853</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>386</v>
@@ -3347,10 +3791,10 @@
         <v>592</v>
       </c>
       <c r="D34" s="1">
-        <v>31287.617466937907</v>
-      </c>
-      <c r="E34" s="1">
-        <v>39825.473470188866</v>
+        <v>40148.47347222222</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>716</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>388</v>
@@ -3372,11 +3816,11 @@
       <c r="C35" t="s">
         <v>593</v>
       </c>
-      <c r="D35" s="1">
-        <v>37677.682838617038</v>
+      <c r="D35" s="1" t="s">
+        <v>717</v>
       </c>
       <c r="E35" s="1">
-        <v>33119.311799293668</v>
+        <v>32941.311793981484</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>390</v>
@@ -3398,11 +3842,11 @@
       <c r="C36" t="s">
         <v>594</v>
       </c>
-      <c r="D36" s="1">
-        <v>38898.98488746061</v>
+      <c r="D36" s="1" t="s">
+        <v>718</v>
       </c>
       <c r="E36" s="1">
-        <v>34640.623028754773</v>
+        <v>34376.623032407406</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>392</v>
@@ -3424,11 +3868,11 @@
       <c r="C37" t="s">
         <v>595</v>
       </c>
-      <c r="D37" s="1">
-        <v>38289.924991781663</v>
+      <c r="D37" s="1" t="s">
+        <v>719</v>
       </c>
       <c r="E37" s="1">
-        <v>34644.649847725064</v>
+        <v>34496.64984953704</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>394</v>
@@ -3450,11 +3894,11 @@
       <c r="C38" t="s">
         <v>596</v>
       </c>
-      <c r="D38" s="1">
-        <v>33043.244504375674</v>
-      </c>
-      <c r="E38" s="1">
-        <v>30922.247305377303</v>
+      <c r="D38" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>721</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>396</v>
@@ -3476,11 +3920,11 @@
       <c r="C39" t="s">
         <v>597</v>
       </c>
-      <c r="D39" s="1">
-        <v>39165.652954820005</v>
-      </c>
-      <c r="E39" s="1">
-        <v>31043.184609155298</v>
+      <c r="D39" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>723</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>398</v>
@@ -3502,11 +3946,11 @@
       <c r="C40" t="s">
         <v>598</v>
       </c>
-      <c r="D40" s="1">
-        <v>33718.301268990079</v>
-      </c>
-      <c r="E40" s="1">
-        <v>33555.789349343082</v>
+      <c r="D40" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>725</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>400</v>
@@ -3528,11 +3972,11 @@
       <c r="C41" t="s">
         <v>599</v>
       </c>
-      <c r="D41" s="1">
-        <v>37702.560137346292</v>
-      </c>
-      <c r="E41" s="1">
-        <v>33721.415616691229</v>
+      <c r="D41" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>727</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>402</v>
@@ -3555,10 +3999,10 @@
         <v>600</v>
       </c>
       <c r="D42" s="1">
-        <v>31965.637332553386</v>
-      </c>
-      <c r="E42" s="1">
-        <v>29572.327829230559</v>
+        <v>31965.637337962962</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>728</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>404</v>
@@ -3580,11 +4024,11 @@
       <c r="C43" t="s">
         <v>601</v>
       </c>
-      <c r="D43" s="1">
-        <v>35058.576187443039</v>
+      <c r="D43" s="1" t="s">
+        <v>729</v>
       </c>
       <c r="E43" s="1">
-        <v>32212.669513337391</v>
+        <v>32419.66951388889</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>406</v>
@@ -3606,11 +4050,11 @@
       <c r="C44" t="s">
         <v>602</v>
       </c>
-      <c r="D44" s="1">
-        <v>36761.478575183442</v>
-      </c>
-      <c r="E44" s="1">
-        <v>34510.161329850052</v>
+      <c r="D44" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>731</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>408</v>
@@ -3633,10 +4077,10 @@
         <v>603</v>
       </c>
       <c r="D45" s="1">
-        <v>29676.531688319141</v>
-      </c>
-      <c r="E45" s="1">
-        <v>36960.470172608533</v>
+        <v>37167.470173611109</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>732</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>410</v>
@@ -3658,11 +4102,11 @@
       <c r="C46" t="s">
         <v>604</v>
       </c>
-      <c r="D46" s="1">
-        <v>31554.177514091291</v>
-      </c>
-      <c r="E46" s="1">
-        <v>29433.348409850027</v>
+      <c r="D46" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>734</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>412</v>
@@ -3685,10 +4129,10 @@
         <v>605</v>
       </c>
       <c r="D47" s="1">
-        <v>35618.68977071163</v>
+        <v>35618.689768518518</v>
       </c>
       <c r="E47" s="1">
-        <v>34213.081409021957</v>
+        <v>33978.081412037034</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>414</v>
@@ -3710,11 +4154,11 @@
       <c r="C48" t="s">
         <v>606</v>
       </c>
-      <c r="D48" s="1">
-        <v>34942.46598134785</v>
+      <c r="D48" s="1" t="s">
+        <v>735</v>
       </c>
       <c r="E48" s="1">
-        <v>32944.854565441114</v>
+        <v>33210.854560185187</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>416</v>
@@ -3736,11 +4180,11 @@
       <c r="C49" t="s">
         <v>607</v>
       </c>
-      <c r="D49" s="1">
-        <v>39405.615950896492</v>
-      </c>
-      <c r="E49" s="1">
-        <v>32776.386956496972</v>
+      <c r="D49" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>737</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>418</v>
@@ -3762,11 +4206,11 @@
       <c r="C50" t="s">
         <v>608</v>
       </c>
-      <c r="D50" s="1">
-        <v>32465.219812298848</v>
-      </c>
-      <c r="E50" s="1">
-        <v>35779.476243483223</v>
+      <c r="D50" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>739</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>420</v>
@@ -3788,11 +4232,11 @@
       <c r="C51" t="s">
         <v>609</v>
       </c>
-      <c r="D51" s="1">
-        <v>33999.478332603518</v>
-      </c>
-      <c r="E51" s="1">
-        <v>33990.095426998967</v>
+      <c r="D51" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>741</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>422</v>
@@ -3815,10 +4259,10 @@
         <v>610</v>
       </c>
       <c r="D52" s="1">
-        <v>35403.808798596066</v>
+        <v>40027.342060185183</v>
       </c>
       <c r="E52" s="1">
-        <v>39852.342064286073</v>
+        <v>35167.808796296296</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>424</v>
@@ -3841,10 +4285,10 @@
         <v>611</v>
       </c>
       <c r="D53" s="1">
-        <v>33408.879819995331</v>
-      </c>
-      <c r="E53" s="1">
-        <v>38723.28827851564</v>
+        <v>38869.288275462961</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>742</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>426</v>
@@ -3867,10 +4311,10 @@
         <v>612</v>
       </c>
       <c r="D54" s="1">
-        <v>34214.200227486399</v>
+        <v>38170.463865740741</v>
       </c>
       <c r="E54" s="1">
-        <v>38024.463870142412</v>
+        <v>34009.200231481482</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>428</v>
@@ -3893,10 +4337,10 @@
         <v>613</v>
       </c>
       <c r="D55" s="1">
-        <v>32119.362781821241</v>
+        <v>38149.945543981485</v>
       </c>
       <c r="E55" s="1">
-        <v>38297.945540021785</v>
+        <v>32001.362777777777</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>430</v>
@@ -3918,11 +4362,11 @@
       <c r="C56" t="s">
         <v>614</v>
       </c>
-      <c r="D56" s="1">
-        <v>37563.678806759955</v>
+      <c r="D56" s="1" t="s">
+        <v>743</v>
       </c>
       <c r="E56" s="1">
-        <v>38153.3489610549</v>
+        <v>37326.678807870368</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>432</v>
@@ -3944,11 +4388,11 @@
       <c r="C57" t="s">
         <v>615</v>
       </c>
-      <c r="D57" s="1">
-        <v>31032.4497835111</v>
-      </c>
-      <c r="E57" s="1">
-        <v>39645.739678413796</v>
+      <c r="D57" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>745</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>434</v>
@@ -3970,11 +4414,11 @@
       <c r="C58" t="s">
         <v>616</v>
       </c>
-      <c r="D58" s="1">
-        <v>39218.378673648607</v>
-      </c>
-      <c r="E58" s="1">
-        <v>31165.995315500069</v>
+      <c r="D58" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>747</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>436</v>
@@ -3997,10 +4441,10 @@
         <v>617</v>
       </c>
       <c r="D59" s="1">
-        <v>34863.813530363564</v>
-      </c>
-      <c r="E59" s="1">
-        <v>39327.980389329779</v>
+        <v>39122.980393518519</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>748</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>438</v>
@@ -4022,11 +4466,11 @@
       <c r="C60" t="s">
         <v>618</v>
       </c>
-      <c r="D60" s="1">
-        <v>39221.408132408571</v>
-      </c>
-      <c r="E60" s="1">
-        <v>36671.417778617702</v>
+      <c r="D60" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>750</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>440</v>
@@ -4048,11 +4492,11 @@
       <c r="C61" t="s">
         <v>619</v>
       </c>
-      <c r="D61" s="1">
-        <v>31643.236519425205</v>
-      </c>
-      <c r="E61" s="1">
-        <v>38651.526095967231</v>
+      <c r="D61" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>752</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>442</v>
@@ -4074,11 +4518,11 @@
       <c r="C62" t="s">
         <v>620</v>
       </c>
-      <c r="D62" s="1">
-        <v>32096.280621487262</v>
-      </c>
-      <c r="E62" s="1">
-        <v>36520.523602276786</v>
+      <c r="D62" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>754</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>444</v>
@@ -4101,10 +4545,10 @@
         <v>621</v>
       </c>
       <c r="D63" s="1">
-        <v>39390.02211985999</v>
+        <v>39183.022118055553</v>
       </c>
       <c r="E63" s="1">
-        <v>31779.872534197108</v>
+        <v>31809.872534722221</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>446</v>
@@ -4126,11 +4570,11 @@
       <c r="C64" t="s">
         <v>622</v>
       </c>
-      <c r="D64" s="1">
-        <v>29987.390656416024</v>
+      <c r="D64" s="1" t="s">
+        <v>755</v>
       </c>
       <c r="E64" s="1">
-        <v>39589.612704290623</v>
+        <v>30073.390659722223</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>448</v>
@@ -4152,11 +4596,11 @@
       <c r="C65" t="s">
         <v>623</v>
       </c>
-      <c r="D65" s="1">
-        <v>38925.79271285906</v>
+      <c r="D65" s="1" t="s">
+        <v>756</v>
       </c>
       <c r="E65" s="1">
-        <v>36626.562726603959</v>
+        <v>36803.562731481485</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>450</v>
@@ -4179,10 +4623,10 @@
         <v>624</v>
       </c>
       <c r="D66" s="1">
-        <v>34680.141081288166</v>
-      </c>
-      <c r="E66" s="1">
-        <v>31892.444685866911</v>
+        <v>34680.141076388885</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>757</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>452</v>
@@ -4204,11 +4648,11 @@
       <c r="C67" t="s">
         <v>625</v>
       </c>
-      <c r="D67" s="1">
-        <v>35486.597365250702</v>
+      <c r="D67" s="1" t="s">
+        <v>758</v>
       </c>
       <c r="E67" s="1">
-        <v>30476.12744011237</v>
+        <v>30565.127442129629</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>454</v>
@@ -4231,10 +4675,10 @@
         <v>626</v>
       </c>
       <c r="D68" s="1">
-        <v>37762.979482056478</v>
-      </c>
-      <c r="E68" s="1">
-        <v>38359.205463409249</v>
+        <v>38534.205462962964</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>759</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>456</v>
@@ -4256,11 +4700,11 @@
       <c r="C69" t="s">
         <v>627</v>
       </c>
-      <c r="D69" s="1">
-        <v>37948.928114798589</v>
-      </c>
-      <c r="E69" s="1">
-        <v>35961.669887842705</v>
+      <c r="D69" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>761</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>458</v>
@@ -4282,11 +4726,11 @@
       <c r="C70" t="s">
         <v>628</v>
       </c>
-      <c r="D70" s="1">
-        <v>36429.726210082437</v>
-      </c>
-      <c r="E70" s="1">
-        <v>34113.339597339786</v>
+      <c r="D70" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>763</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>460</v>
@@ -4309,10 +4753,10 @@
         <v>629</v>
       </c>
       <c r="D71" s="1">
-        <v>29710.312740711539</v>
+        <v>32328.205613425926</v>
       </c>
       <c r="E71" s="1">
-        <v>32240.205615205705</v>
+        <v>29681.312743055554</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>462</v>
@@ -4335,10 +4779,10 @@
         <v>630</v>
       </c>
       <c r="D72" s="1">
-        <v>35070.407637266115</v>
+        <v>37226.230787037035</v>
       </c>
       <c r="E72" s="1">
-        <v>36903.230788314206</v>
+        <v>35217.407638888886</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>464</v>
@@ -4360,11 +4804,11 @@
       <c r="C73" t="s">
         <v>631</v>
       </c>
-      <c r="D73" s="1">
-        <v>39538.624635444408</v>
-      </c>
-      <c r="E73" s="1">
-        <v>34239.818410658998</v>
+      <c r="D73" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>765</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>466</v>
@@ -4386,11 +4830,11 @@
       <c r="C74" t="s">
         <v>632</v>
       </c>
-      <c r="D74" s="1">
-        <v>39532.499633082894</v>
+      <c r="D74" s="1" t="s">
+        <v>766</v>
       </c>
       <c r="E74" s="1">
-        <v>35228.343236004293</v>
+        <v>35405.343240740738</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>468</v>
@@ -4413,10 +4857,10 @@
         <v>633</v>
       </c>
       <c r="D75" s="1">
-        <v>35685.481134244204</v>
-      </c>
-      <c r="E75" s="1">
-        <v>32531.14194698555</v>
+        <v>35773.481134259258</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>767</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>470</v>
@@ -4438,11 +4882,11 @@
       <c r="C76" t="s">
         <v>634</v>
       </c>
-      <c r="D76" s="1">
-        <v>36027.405100632153</v>
-      </c>
-      <c r="E76" s="1">
-        <v>34966.107375379368</v>
+      <c r="D76" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>769</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>472</v>
@@ -4464,11 +4908,11 @@
       <c r="C77" t="s">
         <v>635</v>
       </c>
-      <c r="D77" s="1">
-        <v>40380.212095322124</v>
-      </c>
-      <c r="E77" s="1">
-        <v>30031.553428821095</v>
+      <c r="D77" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>771</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>474</v>
@@ -4490,11 +4934,11 @@
       <c r="C78" t="s">
         <v>636</v>
       </c>
-      <c r="D78" s="1">
-        <v>30396.615963230182</v>
-      </c>
-      <c r="E78" s="1">
-        <v>36915.096150684127</v>
+      <c r="D78" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>773</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>476</v>
@@ -4516,11 +4960,11 @@
       <c r="C79" t="s">
         <v>637</v>
       </c>
-      <c r="D79" s="1">
-        <v>38915.410312730026</v>
-      </c>
-      <c r="E79" s="1">
-        <v>29697.204755349776</v>
+      <c r="D79" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>775</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>478</v>
@@ -4543,10 +4987,10 @@
         <v>638</v>
       </c>
       <c r="D80" s="1">
-        <v>39268.881092662094</v>
+        <v>39209.88108796296</v>
       </c>
       <c r="E80" s="1">
-        <v>35160.942831111897</v>
+        <v>35189.942835648151</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>480</v>
@@ -4569,10 +5013,10 @@
         <v>639</v>
       </c>
       <c r="D81" s="1">
-        <v>39787.817670941855</v>
+        <v>39580.817673611113</v>
       </c>
       <c r="E81" s="1">
-        <v>35318.569348268211</v>
+        <v>35347.569351851853</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>482</v>
@@ -4594,11 +5038,11 @@
       <c r="C82" t="s">
         <v>640</v>
       </c>
-      <c r="D82" s="1">
-        <v>29512.061374950335</v>
-      </c>
-      <c r="E82" s="1">
-        <v>36335.796029682613</v>
+      <c r="D82" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>777</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>484</v>
@@ -4620,11 +5064,11 @@
       <c r="C83" t="s">
         <v>641</v>
       </c>
-      <c r="D83" s="1">
-        <v>31569.902072612767</v>
+      <c r="D83" s="1" t="s">
+        <v>778</v>
       </c>
       <c r="E83" s="1">
-        <v>32795.499855549242</v>
+        <v>31569.902071759258</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>486</v>
@@ -4647,10 +5091,10 @@
         <v>642</v>
       </c>
       <c r="D84" s="1">
-        <v>38840.995896595865</v>
-      </c>
-      <c r="E84" s="1">
-        <v>36422.432298947249</v>
+        <v>38781.995891203704</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>779</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>488</v>
@@ -4672,11 +5116,11 @@
       <c r="C85" t="s">
         <v>643</v>
       </c>
-      <c r="D85" s="1">
-        <v>31356.004752692217</v>
+      <c r="D85" s="1" t="s">
+        <v>780</v>
       </c>
       <c r="E85" s="1">
-        <v>39830.39327308409</v>
+        <v>31178.004756944443</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>490</v>
@@ -4699,10 +5143,10 @@
         <v>644</v>
       </c>
       <c r="D86" s="1">
-        <v>37325.630152537837</v>
+        <v>37532.630150462966</v>
       </c>
       <c r="E86" s="1">
-        <v>32179.443362177542</v>
+        <v>32296.443356481483</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>492</v>
@@ -4724,11 +5168,11 @@
       <c r="C87" t="s">
         <v>645</v>
       </c>
-      <c r="D87" s="1">
-        <v>34814.279429062757</v>
-      </c>
-      <c r="E87" s="1">
-        <v>36906.748382380159</v>
+      <c r="D87" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>782</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>494</v>
@@ -4751,10 +5195,10 @@
         <v>646</v>
       </c>
       <c r="D88" s="1">
-        <v>40036.879821286246</v>
-      </c>
-      <c r="E88" s="1">
-        <v>29325.762342560189</v>
+        <v>40125.879826388889</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>783</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>496</v>
@@ -4777,10 +5221,10 @@
         <v>647</v>
       </c>
       <c r="D89" s="1">
-        <v>37961.616253631037</v>
+        <v>37784.616249999999</v>
       </c>
       <c r="E89" s="1">
-        <v>36503.894739920419</v>
+        <v>36415.894745370373</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>498</v>
@@ -4802,11 +5246,11 @@
       <c r="C90" t="s">
         <v>648</v>
       </c>
-      <c r="D90" s="1">
-        <v>36059.431845237072</v>
-      </c>
-      <c r="E90" s="1">
-        <v>38912.993843379016</v>
+      <c r="D90" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>785</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>500</v>
@@ -4829,10 +5273,10 @@
         <v>649</v>
       </c>
       <c r="D91" s="1">
-        <v>31844.108755336139</v>
-      </c>
-      <c r="E91" s="1">
-        <v>31777.674008239755</v>
+        <v>31992.108749999999</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>786</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>502</v>
@@ -4855,10 +5299,10 @@
         <v>650</v>
       </c>
       <c r="D92" s="1">
-        <v>37812.000458294773</v>
-      </c>
-      <c r="E92" s="1">
-        <v>32375.304412489233</v>
+        <v>37901.000462962962</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>787</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>504</v>
@@ -4880,11 +5324,11 @@
       <c r="C93" t="s">
         <v>651</v>
       </c>
-      <c r="D93" s="1">
-        <v>36446.415013632373</v>
-      </c>
-      <c r="E93" s="1">
-        <v>35934.691127011611</v>
+      <c r="D93" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>789</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>506</v>
@@ -4907,10 +5351,10 @@
         <v>652</v>
       </c>
       <c r="D94" s="1">
-        <v>40089.304676740459</v>
+        <v>39882.304675925923</v>
       </c>
       <c r="E94" s="1">
-        <v>35310.056013513138</v>
+        <v>35104.056018518517</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>508</v>
@@ -4932,11 +5376,11 @@
       <c r="C95" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="1">
-        <v>31643.529283417512</v>
-      </c>
-      <c r="E95" s="1">
-        <v>36430.633859905996</v>
+      <c r="D95" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>791</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>510</v>
@@ -4958,11 +5402,11 @@
       <c r="C96" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="1">
-        <v>33021.39592059877</v>
-      </c>
-      <c r="E96" s="1">
-        <v>31305.273976342192</v>
+      <c r="D96" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>793</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>512</v>
@@ -4984,11 +5428,11 @@
       <c r="C97" t="s">
         <v>655</v>
       </c>
-      <c r="D97" s="1">
-        <v>34633.998775693697</v>
-      </c>
-      <c r="E97" s="1">
-        <v>29964.480242379566</v>
+      <c r="D97" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>795</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>514</v>
@@ -5010,11 +5454,11 @@
       <c r="C98" t="s">
         <v>656</v>
       </c>
-      <c r="D98" s="1">
-        <v>29841.159535820949</v>
+      <c r="D98" s="1" t="s">
+        <v>796</v>
       </c>
       <c r="E98" s="1">
-        <v>35778.099116591584</v>
+        <v>29929.159537037038</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>516</v>
@@ -5036,11 +5480,11 @@
       <c r="C99" t="s">
         <v>657</v>
       </c>
-      <c r="D99" s="1">
-        <v>37064.095718525932</v>
-      </c>
-      <c r="E99" s="1">
-        <v>37400.195488084908</v>
+      <c r="D99" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>798</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>518</v>
@@ -5062,11 +5506,11 @@
       <c r="C100" t="s">
         <v>658</v>
       </c>
-      <c r="D100" s="1">
-        <v>40046.423840871794</v>
+      <c r="D100" s="1" t="s">
+        <v>799</v>
       </c>
       <c r="E100" s="1">
-        <v>36070.167366719295</v>
+        <v>35836.167361111111</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>520</v>
@@ -5088,11 +5532,11 @@
       <c r="C101" t="s">
         <v>659</v>
       </c>
-      <c r="D101" s="1">
-        <v>40110.221552325806</v>
-      </c>
-      <c r="E101" s="1">
-        <v>39293.715080371956</v>
+      <c r="D101" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>801</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>522</v>
@@ -5114,11 +5558,11 @@
       <c r="C102" t="s">
         <v>660</v>
       </c>
-      <c r="D102" s="1">
-        <v>34560.572341727689</v>
-      </c>
-      <c r="E102" s="1">
-        <v>39159.586073222708</v>
+      <c r="D102" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>803</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>524</v>
@@ -5140,11 +5584,11 @@
       <c r="C103" t="s">
         <v>661</v>
       </c>
-      <c r="D103" s="1">
-        <v>34701.387634561863</v>
+      <c r="D103" s="1" t="s">
+        <v>804</v>
       </c>
       <c r="E103" s="1">
-        <v>39775.923879598777</v>
+        <v>34731.387638888889</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>526</v>
@@ -5167,10 +5611,10 @@
         <v>662</v>
       </c>
       <c r="D104" s="1">
-        <v>32967.988865529478</v>
+        <v>32967.988865740743</v>
       </c>
       <c r="E104" s="1">
-        <v>31634.774378224101</v>
+        <v>31693.774375000001</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>528</v>
@@ -5192,11 +5636,11 @@
       <c r="C105" t="s">
         <v>663</v>
       </c>
-      <c r="D105" s="1">
-        <v>39015.528372500106</v>
-      </c>
-      <c r="E105" s="1">
-        <v>36362.523760021271</v>
+      <c r="D105" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>806</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>530</v>
@@ -5218,11 +5662,11 @@
       <c r="C106" t="s">
         <v>664</v>
       </c>
-      <c r="D106" s="1">
-        <v>35525.719582238518</v>
+      <c r="D106" s="1" t="s">
+        <v>807</v>
       </c>
       <c r="E106" s="1">
-        <v>37612.300779799887</v>
+        <v>35554.719583333332</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>532</v>
@@ -5244,11 +5688,11 @@
       <c r="C107" t="s">
         <v>665</v>
       </c>
-      <c r="D107" s="1">
-        <v>32294.419558789559</v>
-      </c>
-      <c r="E107" s="1">
-        <v>29917.174033654952</v>
+      <c r="D107" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>809</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>534</v>
@@ -5270,11 +5714,11 @@
       <c r="C108" t="s">
         <v>666</v>
       </c>
-      <c r="D108" s="1">
-        <v>39774.77764349457</v>
-      </c>
-      <c r="E108" s="1">
-        <v>34414.291479786283</v>
+      <c r="D108" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>811</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>536</v>
@@ -5296,11 +5740,11 @@
       <c r="C109" t="s">
         <v>667</v>
       </c>
-      <c r="D109" s="1">
-        <v>40407.622322833573</v>
-      </c>
-      <c r="E109" s="1">
-        <v>30882.972742469101</v>
+      <c r="D109" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>813</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>538</v>
@@ -5322,11 +5766,11 @@
       <c r="C110" t="s">
         <v>668</v>
       </c>
-      <c r="D110" s="1">
-        <v>36970.772618463328</v>
-      </c>
-      <c r="E110" s="1">
-        <v>37580.035078003246</v>
+      <c r="D110" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>815</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>540</v>
@@ -5349,10 +5793,10 @@
         <v>669</v>
       </c>
       <c r="D111" s="1">
-        <v>30153.828641784985</v>
-      </c>
-      <c r="E111" s="1">
-        <v>33056.123187267964</v>
+        <v>32911.123182870368</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>816</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>542</v>
@@ -5374,11 +5818,11 @@
       <c r="C112" t="s">
         <v>670</v>
       </c>
-      <c r="D112" s="1">
-        <v>33766.813217565781</v>
+      <c r="D112" s="1" t="s">
+        <v>817</v>
       </c>
       <c r="E112" s="1">
-        <v>34841.212205418582</v>
+        <v>33914.813217592593</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>544</v>
@@ -5400,11 +5844,11 @@
       <c r="C113" t="s">
         <v>671</v>
       </c>
-      <c r="D113" s="1">
-        <v>37819.92538134857</v>
-      </c>
-      <c r="E113" s="1">
-        <v>34805.321201821665</v>
+      <c r="D113" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>819</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>546</v>
@@ -5426,11 +5870,11 @@
       <c r="C114" t="s">
         <v>672</v>
       </c>
-      <c r="D114" s="1">
-        <v>34619.491040328518</v>
+      <c r="D114" s="1" t="s">
+        <v>820</v>
       </c>
       <c r="E114" s="1">
-        <v>36692.397681985174</v>
+        <v>34678.491041666668</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>548</v>
@@ -5453,10 +5897,10 @@
         <v>673</v>
       </c>
       <c r="D115" s="1">
-        <v>37895.703801112439</v>
+        <v>37631.703796296293</v>
       </c>
       <c r="E115" s="1">
-        <v>31750.303787885092</v>
+        <v>31514.303784722222</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>550</v>
@@ -5479,10 +5923,10 @@
         <v>674</v>
       </c>
       <c r="D116" s="1">
-        <v>39150.49698955677</v>
+        <v>39328.496990740743</v>
       </c>
       <c r="E116" s="1">
-        <v>35065.480501660357</v>
+        <v>35065.480497685188</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>552</v>
@@ -5504,11 +5948,11 @@
       <c r="C117" t="s">
         <v>675</v>
       </c>
-      <c r="D117" s="1">
-        <v>32901.660951832273</v>
-      </c>
-      <c r="E117" s="1">
-        <v>33594.34344976057</v>
+      <c r="D117" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>822</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>554</v>
@@ -5530,11 +5974,11 @@
       <c r="C118" t="s">
         <v>676</v>
       </c>
-      <c r="D118" s="1">
-        <v>36068.301839377651</v>
+      <c r="D118" s="1" t="s">
+        <v>823</v>
       </c>
       <c r="E118" s="1">
-        <v>29647.711434506462</v>
+        <v>29620.711435185185</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>556</v>
@@ -5556,11 +6000,11 @@
       <c r="C119" t="s">
         <v>677</v>
       </c>
-      <c r="D119" s="1">
-        <v>37094.187032170223</v>
-      </c>
-      <c r="E119" s="1">
-        <v>37649.130398507667</v>
+      <c r="D119" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>825</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>558</v>

</xml_diff>

<commit_message>
Update data file with 'id' field
</commit_message>
<xml_diff>
--- a/quanlythuvien/data/List_DocGia.xlsx
+++ b/quanlythuvien/data/List_DocGia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\Desktop\New folder (2)\mini-library-manager\quanlythuvien\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guest1\Desktop\cn\do an oop\mini-library-manager\quanlythuvien\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9129CEB4-73D7-4658-ACA5-2BCD0A956AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1E63C8-CEBD-41FF-B211-35DBCC563F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3DFCDBD6-3BA2-458F-9082-1DA170B60CF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{3DFCDBD6-3BA2-458F-9082-1DA170B60CF4}"/>
   </bookViews>
   <sheets>
     <sheet name="List_NhanVien" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="827">
   <si>
     <t>username</t>
   </si>
@@ -2521,6 +2520,9 @@
   </si>
   <si>
     <t>22/07/2001 04:29:20</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -2904,3115 +2906,3472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B5E028-7850-4896-8815-10477EF96103}">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>559</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>560</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>88</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>561</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>36080.104930555557</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>680</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>258</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>89</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>562</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>259</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>90</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>563</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>40098.120451388888</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>683</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>260</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>91</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>564</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>30838.082291666666</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>261</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>565</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>34192.376250000001</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>262</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>93</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>566</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>35858.397592592592</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>263</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>94</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>567</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>34983.083078703705</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>32880.500717592593</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>264</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>568</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>687</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>688</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>265</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>96</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>569</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>689</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>690</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>266</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>97</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>570</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>37750.8512962963</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>30107.952928240742</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>267</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>98</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>571</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>35799.335324074076</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>268</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>572</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>33823.85769675926</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>269</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>100</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>573</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>694</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>270</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>101</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>574</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>38412.722361111111</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>695</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>271</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>102</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>575</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>38816.958738425928</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>272</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>103</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>576</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>31087.589479166665</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>273</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>577</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>37046.830057870371</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>30627.820763888889</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>274</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>578</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>33880.041851851849</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>698</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>275</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>106</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>579</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>30992.753391203703</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>29444.004490740739</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>276</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>107</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>580</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>34555.212233796294</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>277</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>108</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>31</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>581</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>39032.373842592591</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>278</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>109</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>582</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>279</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>110</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>583</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>30226.422754629628</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>280</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>111</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>17</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>584</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>281</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>112</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>585</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>35348.964363425926</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>282</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>586</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>707</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>283</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>114</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>35</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>587</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>709</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>710</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>284</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>115</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>36</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>588</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>711</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>36774.874895833331</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>285</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="I30" s="3" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>116</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>589</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>33943.654965277776</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>286</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>6</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>590</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>713</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>714</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>287</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="I32" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>118</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>37</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>591</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>34800.343414351853</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>288</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>119</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>38</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>592</v>
       </c>
-      <c r="D34" s="1">
+      <c r="E34" s="1">
         <v>40148.47347222222</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>716</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>289</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>120</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>39</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>593</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>717</v>
       </c>
-      <c r="E35" s="1">
+      <c r="F35" s="1">
         <v>32941.311793981484</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>290</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>121</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>22</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>594</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="E36" s="1">
+      <c r="F36" s="1">
         <v>34376.623032407406</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>291</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>122</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>22</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>595</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E37" s="1">
+      <c r="F37" s="1">
         <v>34496.64984953704</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>292</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="I37" s="3" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>123</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>596</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>720</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>721</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>293</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="I38" s="3" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>124</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>597</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>723</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>294</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>125</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>42</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>598</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>725</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>295</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="I40" s="3" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>126</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>43</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>599</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>727</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>296</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="I41" s="3" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>127</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>44</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>600</v>
       </c>
-      <c r="D42" s="1">
+      <c r="E42" s="1">
         <v>31965.637337962962</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>728</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>297</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>128</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>44</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>601</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>729</v>
       </c>
-      <c r="E43" s="1">
+      <c r="F43" s="1">
         <v>32419.66951388889</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>298</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="I43" s="3" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>129</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>602</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>730</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>299</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="I44" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>130</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>45</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>603</v>
       </c>
-      <c r="D45" s="1">
+      <c r="E45" s="1">
         <v>37167.470173611109</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>732</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>300</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="I45" s="3" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>131</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>45</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>604</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>733</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>734</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>301</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="I46" s="3" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
         <v>132</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>605</v>
       </c>
-      <c r="D47" s="1">
+      <c r="E47" s="1">
         <v>35618.689768518518</v>
       </c>
-      <c r="E47" s="1">
+      <c r="F47" s="1">
         <v>33978.081412037034</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>302</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="I47" s="3" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>133</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>606</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="1">
         <v>33210.854560185187</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>303</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="I48" s="3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
         <v>134</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>48</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>607</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>736</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>304</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>135</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>49</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>608</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>738</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>739</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>305</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="I50" s="3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>136</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>49</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>609</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>306</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="I51" s="3" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>137</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>49</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>610</v>
       </c>
-      <c r="D52" s="1">
+      <c r="E52" s="1">
         <v>40027.342060185183</v>
       </c>
-      <c r="E52" s="1">
+      <c r="F52" s="1">
         <v>35167.808796296296</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>307</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>138</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>49</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>611</v>
       </c>
-      <c r="D53" s="1">
+      <c r="E53" s="1">
         <v>38869.288275462961</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>308</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="I53" s="3" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>139</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>50</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>612</v>
       </c>
-      <c r="D54" s="1">
+      <c r="E54" s="1">
         <v>38170.463865740741</v>
       </c>
-      <c r="E54" s="1">
+      <c r="F54" s="1">
         <v>34009.200231481482</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>309</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>140</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>51</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>613</v>
       </c>
-      <c r="D55" s="1">
+      <c r="E55" s="1">
         <v>38149.945543981485</v>
       </c>
-      <c r="E55" s="1">
+      <c r="F55" s="1">
         <v>32001.362777777777</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>310</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>141</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>52</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>614</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F56" s="1">
         <v>37326.678807870368</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>311</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="I56" s="3" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>142</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>26</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>615</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>745</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>312</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="I57" s="3" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>143</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>26</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>616</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="G58" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>313</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="I58" s="3" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>144</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>53</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>617</v>
       </c>
-      <c r="D59" s="1">
+      <c r="E59" s="1">
         <v>39122.980393518519</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>314</v>
       </c>
-      <c r="H59" s="3" t="s">
+      <c r="I59" s="3" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>145</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>54</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>618</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>750</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="G60" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>315</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="I60" s="3" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>146</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>55</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>619</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>751</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="G61" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>316</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="I61" s="3" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>147</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>56</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>620</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>753</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="F62" s="2" t="s">
+      <c r="G62" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>317</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="I62" s="3" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>148</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>57</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>621</v>
       </c>
-      <c r="D63" s="1">
+      <c r="E63" s="1">
         <v>39183.022118055553</v>
       </c>
-      <c r="E63" s="1">
+      <c r="F63" s="1">
         <v>31809.872534722221</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>318</v>
       </c>
-      <c r="H63" s="3" t="s">
+      <c r="I63" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>149</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>57</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>622</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>755</v>
       </c>
-      <c r="E64" s="1">
+      <c r="F64" s="1">
         <v>30073.390659722223</v>
       </c>
-      <c r="F64" s="2" t="s">
+      <c r="G64" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>319</v>
       </c>
-      <c r="H64" s="3" t="s">
+      <c r="I64" s="3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
         <v>150</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>58</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>623</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="E65" s="1">
+      <c r="F65" s="1">
         <v>36803.562731481485</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="G65" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>320</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="I65" s="3" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
         <v>151</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>59</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>624</v>
       </c>
-      <c r="D66" s="1">
+      <c r="E66" s="1">
         <v>34680.141076388885</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="F66" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>321</v>
       </c>
-      <c r="H66" s="3" t="s">
+      <c r="I66" s="3" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>152</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>59</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>625</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>758</v>
       </c>
-      <c r="E67" s="1">
+      <c r="F67" s="1">
         <v>30565.127442129629</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>322</v>
       </c>
-      <c r="H67" s="3" t="s">
+      <c r="I67" s="3" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
         <v>153</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>57</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>626</v>
       </c>
-      <c r="D68" s="1">
+      <c r="E68" s="1">
         <v>38534.205462962964</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>759</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="G68" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>205</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="I68" s="3" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
         <v>154</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>8</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>627</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="F69" s="1" t="s">
         <v>761</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>206</v>
       </c>
-      <c r="H69" s="3" t="s">
+      <c r="I69" s="3" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
         <v>155</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>60</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>628</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="F70" s="1" t="s">
         <v>763</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>207</v>
       </c>
-      <c r="H70" s="3" t="s">
+      <c r="I70" s="3" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>156</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>61</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>629</v>
       </c>
-      <c r="D71" s="1">
+      <c r="E71" s="1">
         <v>32328.205613425926</v>
       </c>
-      <c r="E71" s="1">
+      <c r="F71" s="1">
         <v>29681.312743055554</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>208</v>
       </c>
-      <c r="H71" s="3" t="s">
+      <c r="I71" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
         <v>157</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>62</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
         <v>630</v>
       </c>
-      <c r="D72" s="1">
+      <c r="E72" s="1">
         <v>37226.230787037035</v>
       </c>
-      <c r="E72" s="1">
+      <c r="F72" s="1">
         <v>35217.407638888886</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>209</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="I72" s="3" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
         <v>158</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>63</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>631</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>764</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="F73" s="1" t="s">
         <v>765</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>210</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="I73" s="3" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
         <v>159</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>64</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>632</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="E74" s="1" t="s">
         <v>766</v>
       </c>
-      <c r="E74" s="1">
+      <c r="F74" s="1">
         <v>35405.343240740738</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>211</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="I74" s="3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
         <v>160</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>65</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>633</v>
       </c>
-      <c r="D75" s="1">
+      <c r="E75" s="1">
         <v>35773.481134259258</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>212</v>
       </c>
-      <c r="H75" s="3" t="s">
+      <c r="I75" s="3" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>161</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>66</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>634</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F76" s="1" t="s">
         <v>769</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>213</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="I76" s="3" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
         <v>162</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>67</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
         <v>635</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="F77" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>214</v>
       </c>
-      <c r="H77" s="3" t="s">
+      <c r="I77" s="3" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
         <v>163</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>68</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>636</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>773</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>215</v>
       </c>
-      <c r="H78" s="3" t="s">
+      <c r="I78" s="3" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>164</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>69</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>637</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>216</v>
       </c>
-      <c r="H79" s="3" t="s">
+      <c r="I79" s="3" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>165</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>34</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>638</v>
       </c>
-      <c r="D80" s="1">
+      <c r="E80" s="1">
         <v>39209.88108796296</v>
       </c>
-      <c r="E80" s="1">
+      <c r="F80" s="1">
         <v>35189.942835648151</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="G80" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>217</v>
       </c>
-      <c r="H80" s="3" t="s">
+      <c r="I80" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>166</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>67</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>639</v>
       </c>
-      <c r="D81" s="1">
+      <c r="E81" s="1">
         <v>39580.817673611113</v>
       </c>
-      <c r="E81" s="1">
+      <c r="F81" s="1">
         <v>35347.569351851853</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="G81" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>218</v>
       </c>
-      <c r="H81" s="3" t="s">
+      <c r="I81" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
         <v>167</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>70</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>640</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>777</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G82" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>219</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="I82" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
         <v>168</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>7</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>641</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="E83" s="1">
+      <c r="F83" s="1">
         <v>31569.902071759258</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>220</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="I83" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
         <v>169</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>71</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>642</v>
       </c>
-      <c r="D84" s="1">
+      <c r="E84" s="1">
         <v>38781.995891203704</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>221</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="I84" s="3" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
         <v>170</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>64</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>643</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="E85" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="E85" s="1">
+      <c r="F85" s="1">
         <v>31178.004756944443</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>222</v>
       </c>
-      <c r="H85" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
         <v>171</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>72</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>644</v>
       </c>
-      <c r="D86" s="1">
+      <c r="E86" s="1">
         <v>37532.630150462966</v>
       </c>
-      <c r="E86" s="1">
+      <c r="F86" s="1">
         <v>32296.443356481483</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>223</v>
       </c>
-      <c r="H86" s="3" t="s">
+      <c r="I86" s="3" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
         <v>172</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>10</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>645</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>224</v>
       </c>
-      <c r="H87" s="3" t="s">
+      <c r="I87" s="3" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
         <v>173</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>73</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>646</v>
       </c>
-      <c r="D88" s="1">
+      <c r="E88" s="1">
         <v>40125.879826388889</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>225</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="I88" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
         <v>174</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>74</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>647</v>
       </c>
-      <c r="D89" s="1">
+      <c r="E89" s="1">
         <v>37784.616249999999</v>
       </c>
-      <c r="E89" s="1">
+      <c r="F89" s="1">
         <v>36415.894745370373</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="G89" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>226</v>
       </c>
-      <c r="H89" s="3" t="s">
+      <c r="I89" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
         <v>175</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>12</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>648</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="E90" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>227</v>
       </c>
-      <c r="H90" s="3" t="s">
+      <c r="I90" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
         <v>176</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>67</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>649</v>
       </c>
-      <c r="D91" s="1">
+      <c r="E91" s="1">
         <v>31992.108749999999</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>228</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="I91" s="3" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
         <v>177</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>8</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>650</v>
       </c>
-      <c r="D92" s="1">
+      <c r="E92" s="1">
         <v>37901.000462962962</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>229</v>
       </c>
-      <c r="H92" s="3" t="s">
+      <c r="I92" s="3" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
         <v>178</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>651</v>
       </c>
-      <c r="D93" s="1" t="s">
+      <c r="E93" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>230</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="I93" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
         <v>179</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>75</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>652</v>
       </c>
-      <c r="D94" s="1">
+      <c r="E94" s="1">
         <v>39882.304675925923</v>
       </c>
-      <c r="E94" s="1">
+      <c r="F94" s="1">
         <v>35104.056018518517</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="G94" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>231</v>
       </c>
-      <c r="H94" s="3" t="s">
+      <c r="I94" s="3" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
         <v>180</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>70</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>653</v>
       </c>
-      <c r="D95" s="1" t="s">
+      <c r="E95" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="G95" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>232</v>
       </c>
-      <c r="H95" s="3" t="s">
+      <c r="I95" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
         <v>181</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>9</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>654</v>
       </c>
-      <c r="D96" s="1" t="s">
+      <c r="E96" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="G96" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>233</v>
       </c>
-      <c r="H96" s="3" t="s">
+      <c r="I96" s="3" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
         <v>182</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>76</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>655</v>
       </c>
-      <c r="D97" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="G97" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>234</v>
       </c>
-      <c r="H97" s="3" t="s">
+      <c r="I97" s="3" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
         <v>183</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>75</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>656</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="E98" s="1">
+      <c r="F98" s="1">
         <v>29929.159537037038</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>235</v>
       </c>
-      <c r="H98" s="3" t="s">
+      <c r="I98" s="3" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
         <v>184</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>10</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>657</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="E99" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="G99" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>236</v>
       </c>
-      <c r="H99" s="3" t="s">
+      <c r="I99" s="3" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
         <v>185</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>68</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
         <v>658</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="E100" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="E100" s="1">
+      <c r="F100" s="1">
         <v>35836.167361111111</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="G100" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>237</v>
       </c>
-      <c r="H100" s="3" t="s">
+      <c r="I100" s="3" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
         <v>186</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>51</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>659</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="G101" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>238</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="I101" s="3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
         <v>187</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>64</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>660</v>
       </c>
-      <c r="D102" s="1" t="s">
+      <c r="E102" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="F102" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>239</v>
       </c>
-      <c r="H102" s="3" t="s">
+      <c r="I102" s="3" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
         <v>188</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>77</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>661</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="E103" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="E103" s="1">
+      <c r="F103" s="1">
         <v>34731.387638888889</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="G103" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>240</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="I103" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
         <v>189</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>78</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>662</v>
       </c>
-      <c r="D104" s="1">
+      <c r="E104" s="1">
         <v>32967.988865740743</v>
       </c>
-      <c r="E104" s="1">
+      <c r="F104" s="1">
         <v>31693.774375000001</v>
       </c>
-      <c r="F104" s="2" t="s">
+      <c r="G104" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" t="s">
         <v>241</v>
       </c>
-      <c r="H104" s="3" t="s">
+      <c r="I104" s="3" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
         <v>190</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>79</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>663</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>805</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="G105" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>242</v>
       </c>
-      <c r="H105" s="3" t="s">
+      <c r="I105" s="3" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
         <v>191</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>80</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
         <v>664</v>
       </c>
-      <c r="D106" s="1" t="s">
+      <c r="E106" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="E106" s="1">
+      <c r="F106" s="1">
         <v>35554.719583333332</v>
       </c>
-      <c r="F106" s="2" t="s">
+      <c r="G106" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="G106" t="s">
+      <c r="H106" t="s">
         <v>243</v>
       </c>
-      <c r="H106" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
         <v>192</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>81</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>665</v>
       </c>
-      <c r="D107" s="1" t="s">
+      <c r="E107" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="F107" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="G107" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>244</v>
       </c>
-      <c r="H107" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
         <v>193</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>82</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>666</v>
       </c>
-      <c r="D108" s="1" t="s">
+      <c r="E108" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="F108" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="G108" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>245</v>
       </c>
-      <c r="H108" s="3" t="s">
+      <c r="I108" s="3" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
         <v>194</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>10</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>667</v>
       </c>
-      <c r="D109" s="1" t="s">
+      <c r="E109" s="1" t="s">
         <v>812</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="F109" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="F109" s="2" t="s">
+      <c r="G109" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>246</v>
       </c>
-      <c r="H109" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
         <v>195</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>83</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>668</v>
       </c>
-      <c r="D110" s="1" t="s">
+      <c r="E110" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="F110" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>247</v>
       </c>
-      <c r="H110" s="3" t="s">
+      <c r="I110" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
         <v>196</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>70</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>669</v>
       </c>
-      <c r="D111" s="1">
+      <c r="E111" s="1">
         <v>32911.123182870368</v>
       </c>
-      <c r="E111" s="1" t="s">
+      <c r="F111" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>248</v>
       </c>
-      <c r="H111" s="3" t="s">
+      <c r="I111" s="3" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
         <v>197</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>74</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>670</v>
       </c>
-      <c r="D112" s="1" t="s">
+      <c r="E112" s="1" t="s">
         <v>817</v>
       </c>
-      <c r="E112" s="1">
+      <c r="F112" s="1">
         <v>33914.813217592593</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="G112" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>249</v>
       </c>
-      <c r="H112" s="3" t="s">
+      <c r="I112" s="3" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
         <v>198</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>84</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>671</v>
       </c>
-      <c r="D113" s="1" t="s">
+      <c r="E113" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="F113" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="G113" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="G113" t="s">
+      <c r="H113" t="s">
         <v>250</v>
       </c>
-      <c r="H113" s="3" t="s">
+      <c r="I113" s="3" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
         <v>199</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>85</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>672</v>
       </c>
-      <c r="D114" s="1" t="s">
+      <c r="E114" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="E114" s="1">
+      <c r="F114" s="1">
         <v>34678.491041666668</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="G114" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>251</v>
       </c>
-      <c r="H114" s="3" t="s">
+      <c r="I114" s="3" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
         <v>200</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>84</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>673</v>
       </c>
-      <c r="D115" s="1">
+      <c r="E115" s="1">
         <v>37631.703796296293</v>
       </c>
-      <c r="E115" s="1">
+      <c r="F115" s="1">
         <v>31514.303784722222</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="G115" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="G115" t="s">
+      <c r="H115" t="s">
         <v>252</v>
       </c>
-      <c r="H115" s="3" t="s">
+      <c r="I115" s="3" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
         <v>201</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>68</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>674</v>
       </c>
-      <c r="D116" s="1">
+      <c r="E116" s="1">
         <v>39328.496990740743</v>
       </c>
-      <c r="E116" s="1">
+      <c r="F116" s="1">
         <v>35065.480497685188</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="G116" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="G116" t="s">
+      <c r="H116" t="s">
         <v>253</v>
       </c>
-      <c r="H116" s="3" t="s">
+      <c r="I116" s="3" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
         <v>202</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>34</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>675</v>
       </c>
-      <c r="D117" s="1" t="s">
+      <c r="E117" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="E117" s="1" t="s">
+      <c r="F117" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="G117" t="s">
+      <c r="H117" t="s">
         <v>254</v>
       </c>
-      <c r="H117" s="3" t="s">
+      <c r="I117" s="3" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
         <v>203</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>86</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>676</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="E118" s="1">
+      <c r="F118" s="1">
         <v>29620.711435185185</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="G118" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
         <v>255</v>
       </c>
-      <c r="H118" s="3" t="s">
+      <c r="I118" s="3" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
         <v>204</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>11</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>677</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="E119" s="1" t="s">
+      <c r="F119" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="G119" t="s">
+      <c r="H119" t="s">
         <v>256</v>
       </c>
-      <c r="H119" s="3" t="s">
+      <c r="I119" s="3" t="s">
         <v>557</v>
       </c>
     </row>

</xml_diff>